<commit_message>
Add cmd entry of how to make a network shared folder
</commit_message>
<xml_diff>
--- a/cmd_lib.xlsx
+++ b/cmd_lib.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,12 +11,12 @@
     <sheet name="工作表2" sheetId="2" r:id="rId2"/>
     <sheet name="工作表3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>window OS</t>
   </si>
@@ -47,16 +47,27 @@
   <si>
     <t>CODE</t>
   </si>
+  <si>
+    <t>network</t>
+  </si>
+  <si>
+    <t>make a network share drive</t>
+  </si>
+  <si>
+    <t>1. Folder right click &gt; properties &gt; sharing tab &gt; share &gt; add everyone to write/read
+2. &gt;net use a: \\pc-011-032\drivea
+3. &gt;net use     **this can check whether the new netowrk shared folder is activated</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -67,7 +78,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -109,13 +120,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -128,7 +142,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -202,7 +216,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -237,7 +250,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -413,21 +425,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="10.25" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
     <col min="3" max="3" width="73" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -438,7 +450,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -449,7 +461,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -458,6 +470,17 @@
       </c>
       <c r="C3" s="1" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="47.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -467,12 +490,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -480,12 +503,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>